<commit_message>
Begin multi user version
Add new shema data base
Add new sql function
Add some reaction
All in process...
</commit_message>
<xml_diff>
--- a/nnm_tables.xlsx
+++ b/nnm_tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t xml:space="preserve">FILMS</t>
   </si>
@@ -106,46 +106,70 @@
     <t xml:space="preserve">rights</t>
   </si>
   <si>
+    <t xml:space="preserve">id user in telegram primary key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id film on kinopoisk.ru site</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">TEXT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PK</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">name user in telegram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id film on imdb .org site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">katerina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date add user in database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date add film in database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activ or no user (blocked)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tag for download film or untag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rights of  user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFILMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_FILMS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Primary key auto increment</t>
   </si>
   <si>
-    <t xml:space="preserve">id film on kinopoisk.ru site</t>
-  </si>
-  <si>
     <t xml:space="preserve">INT  PKAI</t>
   </si>
   <si>
     <t xml:space="preserve">id user in telegram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id film on imdb .org site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">katerina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name user in telegram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date add film in database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date add user in database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tag for download film or untag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activ or no user (blocked)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rights of  user </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UFILMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_FILMS</t>
   </si>
   <si>
     <t xml:space="preserve">id film in table FILMS-id</t>
@@ -165,7 +189,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,8 +248,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,12 +278,6 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.1"/>
         <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF860D"/>
-        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -314,7 +338,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,28 +403,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -475,7 +487,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF860D"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -671,8 +683,8 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,7 +696,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="7.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="35.57"/>
   </cols>
@@ -826,152 +838,139 @@
         <v>23</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7" t="s">
+      <c r="H6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
-      <c r="B8" s="21" t="n">
+      <c r="B8" s="11" t="n">
+        <v>25333560</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>38276</v>
+      </c>
+      <c r="E8" s="10" t="n">
         <v>1</v>
-      </c>
-      <c r="C8" s="11" t="n">
-        <v>25333560</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="14" t="n">
-        <v>38276</v>
       </c>
       <c r="F8" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="H8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="7" t="s">
+      <c r="H9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="7" t="s">
+      <c r="H10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="19" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -981,15 +980,15 @@
         <v>1</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -998,38 +997,38 @@
       <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23" t="n">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="24" t="n">
+      <c r="C16" s="21" t="n">
         <v>25333560</v>
       </c>
-      <c r="D16" s="24" t="n">
+      <c r="D16" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="E16" s="25" t="n">
+      <c r="E16" s="22" t="n">
         <v>45348</v>
       </c>
-      <c r="F16" s="23" t="n">
+      <c r="F16" s="20" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,15 +1039,15 @@
         <v>8</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="19" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>